<commit_message>
Added V1 VendorOrder Order Creation
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4128" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4128" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VendorTripCreation" sheetId="1" r:id="rId1"/>
     <sheet name="Dotpe" sheetId="2" r:id="rId2"/>
+    <sheet name="v1VendorOrder" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>TestCases</t>
   </si>
@@ -253,6 +254,30 @@
   </si>
   <si>
     <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>v1VendorOrderTripCreation</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <t>ABChihi</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>cash_to_be_collected</t>
+  </si>
+  <si>
+    <t>21:00-22:00</t>
   </si>
 </sst>
 </file>
@@ -288,8 +313,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
@@ -774,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection sqref="A1:AR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,4 +1003,237 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" customWidth="1"/>
+    <col min="16" max="16" width="19" customWidth="1"/>
+    <col min="17" max="17" width="23.109375" customWidth="1"/>
+    <col min="18" max="18" width="34.33203125" customWidth="1"/>
+    <col min="19" max="19" width="34.6640625" customWidth="1"/>
+    <col min="20" max="20" width="25.77734375" customWidth="1"/>
+    <col min="21" max="21" width="28.109375" customWidth="1"/>
+    <col min="22" max="22" width="17.77734375" customWidth="1"/>
+    <col min="23" max="23" width="19.88671875" customWidth="1"/>
+    <col min="24" max="24" width="19" customWidth="1"/>
+    <col min="25" max="25" width="29.21875" customWidth="1"/>
+    <col min="26" max="26" width="26.33203125" customWidth="1"/>
+    <col min="27" max="27" width="32.21875" customWidth="1"/>
+    <col min="28" max="28" width="37.33203125" customWidth="1"/>
+    <col min="29" max="29" width="22.33203125" customWidth="1"/>
+    <col min="30" max="30" width="22.77734375" customWidth="1"/>
+    <col min="31" max="31" width="21.21875" customWidth="1"/>
+    <col min="32" max="32" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="E2">
+        <v>900</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2">
+        <v>9839864601</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2">
+        <v>9911561689</v>
+      </c>
+      <c r="M2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2">
+        <v>9919809990</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T2">
+        <v>28.6295</v>
+      </c>
+      <c r="U2">
+        <v>77.077799999999996</v>
+      </c>
+      <c r="V2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2">
+        <v>110058</v>
+      </c>
+      <c r="X2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC2">
+        <v>28.5747</v>
+      </c>
+      <c r="AD2">
+        <v>77.355999999999995</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF2">
+        <v>201301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>